<commit_message>
Se termina el envio de Notificaciones
</commit_message>
<xml_diff>
--- a/Pendientes.xlsx
+++ b/Pendientes.xlsx
@@ -226,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,12 +260,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,15 +302,15 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +606,7 @@
     <col min="6" max="6" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -647,27 +641,27 @@
         <v>8</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="H3" s="9"/>
+      <c r="H3" s="7"/>
       <c r="I3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="H4" s="11"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="H4" s="9"/>
       <c r="I4" t="s">
         <v>58</v>
       </c>
@@ -687,7 +681,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="H5" s="10"/>
+      <c r="H5" s="8"/>
       <c r="I5" t="s">
         <v>59</v>
       </c>
@@ -839,7 +833,7 @@
       <c r="E13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -859,7 +853,7 @@
       <c r="E14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1054,20 +1048,20 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="11">
         <v>23</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="8" t="s">
+      <c r="D25" s="11"/>
+      <c r="E25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Subo los cambios para atender las observaciones sobre los saldos vacacionales, asi como los 3 nuevos reportes.
</commit_message>
<xml_diff>
--- a/Pendientes.xlsx
+++ b/Pendientes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos Quality\IICA\sia_icca\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@Freelance\@IICA\Proyectos\Permisos_Vacaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E0E68A-D38C-41C9-8956-8ECB9D14800A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25890" windowHeight="10215"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>Folio</t>
   </si>
@@ -204,12 +205,15 @@
   </si>
   <si>
     <t>oscarin</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -226,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +279,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -288,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -308,15 +318,18 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,11 +609,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +625,7 @@
     <col min="6" max="6" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -647,7 +660,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="H3" s="9"/>
+      <c r="H3" s="8"/>
       <c r="I3" t="s">
         <v>57</v>
       </c>
@@ -667,7 +680,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="H4" s="11"/>
+      <c r="H4" s="10"/>
       <c r="I4" t="s">
         <v>58</v>
       </c>
@@ -687,7 +700,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="H5" s="10"/>
+      <c r="H5" s="9"/>
       <c r="I5" t="s">
         <v>59</v>
       </c>
@@ -705,8 +718,8 @@
       <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>8</v>
+      <c r="E6" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>54</v>
@@ -780,8 +793,8 @@
       <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>8</v>
+      <c r="E10" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>47</v>
@@ -836,10 +849,10 @@
       <c r="D13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="7" t="s">
+      <c r="E13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>48</v>
       </c>
     </row>
@@ -856,10 +869,10 @@
       <c r="D14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="7"/>
+      <c r="E14" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -892,8 +905,8 @@
         <v>32</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="6" t="s">
-        <v>8</v>
+      <c r="E16" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>51</v>
@@ -930,8 +943,8 @@
       <c r="D18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>8</v>
+      <c r="E18" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>52</v>
@@ -989,8 +1002,8 @@
       <c r="D21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>8</v>
+      <c r="E21" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>53</v>
@@ -1009,8 +1022,8 @@
       <c r="D22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>8</v>
+      <c r="E22" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>54</v>
@@ -1067,7 +1080,7 @@
       <c r="E25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="7" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizo el status de las incidencias.
</commit_message>
<xml_diff>
--- a/Pendientes.xlsx
+++ b/Pendientes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos Quality\IICA\sia_icca\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@Freelance\@IICA\Proyectos\Permisos_Vacaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667469E2-340C-409F-8155-C53C67903120}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25890" windowHeight="10215"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="61">
   <si>
     <t>Folio</t>
   </si>
@@ -204,12 +205,15 @@
   </si>
   <si>
     <t>oscarin</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -226,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +273,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -308,8 +318,8 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,11 +600,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,8 +709,8 @@
       <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>8</v>
+      <c r="E6" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>54</v>
@@ -774,8 +784,8 @@
       <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>8</v>
+      <c r="E10" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>47</v>
@@ -830,8 +840,8 @@
       <c r="D13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>8</v>
+      <c r="E13" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>48</v>
@@ -850,8 +860,8 @@
       <c r="D14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>8</v>
+      <c r="E14" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F14" s="10"/>
     </row>
@@ -886,8 +896,8 @@
         <v>32</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="6" t="s">
-        <v>8</v>
+      <c r="E16" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>51</v>
@@ -924,8 +934,8 @@
       <c r="D18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>8</v>
+      <c r="E18" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>52</v>
@@ -983,8 +993,8 @@
       <c r="D21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>8</v>
+      <c r="E21" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>53</v>
@@ -1003,8 +1013,8 @@
       <c r="D22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>8</v>
+      <c r="E22" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>54</v>
@@ -1048,20 +1058,20 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="11" t="s">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>